<commit_message>
TEMP: FIX TESTS (ainakin kieli viel uppercase)
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku.xlsx
+++ b/src/test/resources/erillishaku.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Rakennusalan perustutkinto</t>
   </si>
@@ -34,7 +34,13 @@
     <t>Syntymäaika</t>
   </si>
   <si>
+    <t>Sukupuoli</t>
+  </si>
+  <si>
     <t>Hakija-oid</t>
+  </si>
+  <si>
+    <t>Äidinkieli</t>
   </si>
   <si>
     <t>Hakemuksentila</t>
@@ -70,6 +76,12 @@
   </si>
   <si>
     <t>1.1.1901</t>
+  </si>
+  <si>
+    <t>MIES</t>
+  </si>
+  <si>
+    <t>FI</t>
   </si>
   <si>
     <t>HYVAKSYTTY</t>
@@ -1467,7 +1479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1483,7 +1495,9 @@
     <col min="8" max="8" width="8.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.125" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.125" style="1" customWidth="1"/>
-    <col min="11" max="256" width="8.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.125" style="1" customWidth="1"/>
+    <col min="13" max="256" width="8.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1">
@@ -1497,6 +1511,8 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" ht="14" customHeight="1">
       <c r="A2" t="s" s="6">
@@ -1511,6 +1527,8 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" ht="14" customHeight="1">
       <c r="A3" t="s" s="6">
@@ -1525,6 +1543,8 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" s="5"/>
@@ -1537,6 +1557,8 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" ht="14" customHeight="1">
       <c r="A5" t="s" s="7">
@@ -1569,35 +1591,47 @@
       <c r="J5" t="s" s="7">
         <v>11</v>
       </c>
+      <c r="K5" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s" s="7">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" ht="14" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s" s="7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" t="s" s="7">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5"/>
       <c r="H6" t="s" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s" s="7">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s" s="7">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K6" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s" s="7">
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="17" customHeight="1">
@@ -1611,6 +1645,8 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="5"/>
@@ -1623,6 +1659,8 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="5"/>
@@ -1635,6 +1673,8 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="5"/>
@@ -1647,6 +1687,8 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fix tests for excel import
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku.xlsx
+++ b/src/test/resources/erillishaku.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petur1/git/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommi.helander/src/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38320" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260"/>
   </bookViews>
   <sheets>
     <sheet name="Erillishaku" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Rakennusalan perustutkinto</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Ei</t>
+  </si>
+  <si>
+    <t>Hyväksymisen ehto</t>
   </si>
 </sst>
 </file>
@@ -1553,18 +1556,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="257" width="8.125" style="1" customWidth="1"/>
+    <col min="1" max="9" width="8.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="1" customWidth="1"/>
+    <col min="13" max="14" width="8.125" style="1" customWidth="1"/>
+    <col min="15" max="258" width="8.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1578,8 +1586,9 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1595,8 +1604,9 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1612,8 +1622,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1627,8 +1638,9 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1660,16 +1672,19 @@
         <v>24</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1698,17 +1713,18 @@
       <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="M6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1722,8 +1738,9 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1737,8 +1754,9 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1752,8 +1770,9 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1767,6 +1786,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>